<commit_message>
Add page link into the table
</commit_message>
<xml_diff>
--- a/TAF_EasyRest/TestFramework/page_links.xlsx
+++ b/TAF_EasyRest/TestFramework/page_links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Page</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>/restaurants</t>
+  </si>
+  <si>
+    <t>ModeratorPanelRestaurantsPage</t>
+  </si>
+  <si>
+    <t>/moderator/restaurants</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -477,6 +483,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>14</v>

</xml_diff>